<commit_message>
minor changes in inline
</commit_message>
<xml_diff>
--- a/backend/templates/Inline-inspection-form.xlsx
+++ b/backend/templates/Inline-inspection-form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cursor AI Projects\SwansonIndiaPortal\backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5236185-F224-4F56-83C2-7684148035A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BCBA11-D270-4BFC-BB45-592FC845856D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="588" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -739,20 +739,8 @@
     <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -760,11 +748,8 @@
     <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -772,35 +757,29 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -814,56 +793,14 @@
     <xf numFmtId="2" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -904,28 +841,94 @@
     <xf numFmtId="49" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -933,9 +936,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1271,10 +1271,10 @@
         <v>0</v>
       </c>
       <c r="AD1" s="3"/>
-      <c r="AE1" s="97" t="s">
+      <c r="AE1" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="AF1" s="97"/>
+      <c r="AF1" s="42"/>
       <c r="AI1" s="4"/>
       <c r="AJ1" s="4"/>
       <c r="AK1" s="4"/>
@@ -1285,230 +1285,228 @@
       <c r="A2" s="5"/>
       <c r="AC2" s="6"/>
       <c r="AD2" s="6"/>
-      <c r="AE2" s="104" t="s">
+      <c r="AE2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="AF2" s="104"/>
+      <c r="AF2" s="39"/>
     </row>
     <row r="3" spans="1:39" s="7" customFormat="1" ht="26.25">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="98"/>
-      <c r="R3" s="98"/>
-      <c r="S3" s="98"/>
-      <c r="T3" s="98"/>
-      <c r="U3" s="98"/>
-      <c r="V3" s="98"/>
-      <c r="W3" s="98"/>
-      <c r="X3" s="98"/>
-      <c r="Y3" s="98"/>
-      <c r="Z3" s="98"/>
-      <c r="AA3" s="98"/>
-      <c r="AB3" s="98"/>
-      <c r="AC3" s="98"/>
-      <c r="AD3" s="98"/>
-      <c r="AE3" s="98"/>
-      <c r="AF3" s="98"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="47"/>
+      <c r="Z3" s="47"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="47"/>
+      <c r="AC3" s="47"/>
+      <c r="AD3" s="47"/>
+      <c r="AE3" s="47"/>
+      <c r="AF3" s="47"/>
     </row>
     <row r="4" spans="1:39" s="8" customFormat="1" ht="19.5">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
-      <c r="N4" s="99"/>
-      <c r="O4" s="99"/>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="99"/>
-      <c r="V4" s="99"/>
-      <c r="W4" s="99"/>
-      <c r="X4" s="99"/>
-      <c r="Y4" s="99"/>
-      <c r="Z4" s="99"/>
-      <c r="AA4" s="99"/>
-      <c r="AB4" s="99"/>
-      <c r="AC4" s="99"/>
-      <c r="AD4" s="99"/>
-      <c r="AE4" s="99"/>
-      <c r="AF4" s="99"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="48"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="48"/>
+      <c r="AD4" s="48"/>
+      <c r="AE4" s="48"/>
+      <c r="AF4" s="48"/>
     </row>
     <row r="5" spans="1:39" s="9" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="AC5" s="100"/>
-      <c r="AD5" s="100"/>
-      <c r="AE5" s="101"/>
-      <c r="AF5" s="101"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="49"/>
+      <c r="AE5" s="50"/>
+      <c r="AF5" s="50"/>
     </row>
     <row r="6" spans="1:39" s="9" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="93"/>
+      <c r="H6" s="93"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="53" t="s">
+      <c r="J6" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="53"/>
+      <c r="K6" s="46"/>
       <c r="L6" s="11"/>
-      <c r="N6" s="44" t="s">
+      <c r="N6" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="45"/>
-      <c r="P6" s="44" t="s">
+      <c r="O6" s="41"/>
+      <c r="P6" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="44" t="s">
+      <c r="Q6" s="41"/>
+      <c r="R6" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="45"/>
-      <c r="T6" s="44" t="s">
+      <c r="S6" s="41"/>
+      <c r="T6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="U6" s="45"/>
-      <c r="V6" s="44" t="s">
+      <c r="U6" s="41"/>
+      <c r="V6" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="W6" s="45"/>
-      <c r="AB6" s="48" t="s">
+      <c r="W6" s="41"/>
+      <c r="AB6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="AC6" s="48"/>
-      <c r="AD6" s="49"/>
-      <c r="AE6" s="46"/>
-      <c r="AF6" s="47"/>
+      <c r="AC6" s="43"/>
+      <c r="AD6" s="44"/>
+      <c r="AE6" s="98"/>
+      <c r="AF6" s="99"/>
     </row>
     <row r="7" spans="1:39" s="10" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="J7" s="53" t="s">
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="J7" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="49"/>
+      <c r="K7" s="44"/>
       <c r="L7" s="11"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="40"/>
-      <c r="V7" s="39"/>
-      <c r="W7" s="40"/>
-      <c r="AB7" s="48" t="s">
+      <c r="N7" s="94"/>
+      <c r="O7" s="95"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="95"/>
+      <c r="R7" s="94"/>
+      <c r="S7" s="95"/>
+      <c r="T7" s="94"/>
+      <c r="U7" s="95"/>
+      <c r="V7" s="94"/>
+      <c r="W7" s="95"/>
+      <c r="AB7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="AC7" s="48"/>
-      <c r="AD7" s="49"/>
-      <c r="AE7" s="50">
-        <v>1</v>
-      </c>
-      <c r="AF7" s="51"/>
+      <c r="AC7" s="43"/>
+      <c r="AD7" s="44"/>
+      <c r="AE7" s="100"/>
+      <c r="AF7" s="101"/>
     </row>
     <row r="8" spans="1:39" s="9" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="J8" s="53" t="s">
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="J8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="53"/>
+      <c r="K8" s="46"/>
       <c r="L8" s="11"/>
       <c r="M8" s="10"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="41"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="41"/>
-      <c r="U8" s="42"/>
-      <c r="V8" s="41"/>
-      <c r="W8" s="42"/>
+      <c r="N8" s="96"/>
+      <c r="O8" s="97"/>
+      <c r="P8" s="96"/>
+      <c r="Q8" s="97"/>
+      <c r="R8" s="96"/>
+      <c r="S8" s="97"/>
+      <c r="T8" s="96"/>
+      <c r="U8" s="97"/>
+      <c r="V8" s="96"/>
+      <c r="W8" s="97"/>
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
       <c r="AA8" s="10"/>
-      <c r="AB8" s="48" t="s">
+      <c r="AB8" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="AC8" s="48"/>
-      <c r="AD8" s="49"/>
-      <c r="AE8" s="102"/>
-      <c r="AF8" s="103"/>
+      <c r="AC8" s="43"/>
+      <c r="AD8" s="44"/>
+      <c r="AE8" s="103"/>
+      <c r="AF8" s="104"/>
     </row>
     <row r="9" spans="1:39" s="9" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
       <c r="L9" s="37"/>
       <c r="M9" s="36"/>
       <c r="N9" s="38"/>
@@ -1525,61 +1523,61 @@
       <c r="Y9" s="36"/>
       <c r="Z9" s="36"/>
       <c r="AA9" s="36"/>
-      <c r="AB9" s="53"/>
-      <c r="AC9" s="53"/>
-      <c r="AD9" s="53"/>
-      <c r="AE9" s="43"/>
-      <c r="AF9" s="43"/>
+      <c r="AB9" s="46"/>
+      <c r="AC9" s="46"/>
+      <c r="AD9" s="46"/>
+      <c r="AE9" s="102"/>
+      <c r="AF9" s="102"/>
     </row>
     <row r="10" spans="1:39" s="9" customFormat="1" ht="6" customHeight="1">
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="90"/>
+      <c r="L10" s="90"/>
     </row>
     <row r="11" spans="1:39" s="17" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="58" t="s">
+      <c r="B11" s="78"/>
+      <c r="C11" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="59"/>
+      <c r="H11" s="92"/>
       <c r="I11" s="13"/>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="59"/>
+      <c r="K11" s="92"/>
       <c r="L11" s="13"/>
-      <c r="M11" s="56" t="s">
+      <c r="M11" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="73"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
-      <c r="R11" s="73"/>
-      <c r="S11" s="73"/>
-      <c r="T11" s="73"/>
-      <c r="U11" s="73"/>
-      <c r="V11" s="73"/>
-      <c r="W11" s="73"/>
-      <c r="X11" s="73"/>
-      <c r="Y11" s="73"/>
-      <c r="Z11" s="73"/>
-      <c r="AA11" s="73"/>
-      <c r="AB11" s="57"/>
-      <c r="AC11" s="74" t="s">
+      <c r="N11" s="77"/>
+      <c r="O11" s="77"/>
+      <c r="P11" s="77"/>
+      <c r="Q11" s="77"/>
+      <c r="R11" s="77"/>
+      <c r="S11" s="77"/>
+      <c r="T11" s="77"/>
+      <c r="U11" s="77"/>
+      <c r="V11" s="77"/>
+      <c r="W11" s="77"/>
+      <c r="X11" s="77"/>
+      <c r="Y11" s="77"/>
+      <c r="Z11" s="77"/>
+      <c r="AA11" s="77"/>
+      <c r="AB11" s="78"/>
+      <c r="AC11" s="79" t="s">
         <v>19</v>
       </c>
       <c r="AD11" s="14" t="s">
@@ -1588,75 +1586,75 @@
       <c r="AE11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="AF11" s="64" t="s">
+      <c r="AF11" s="84" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:39" s="20" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="65" t="s">
+      <c r="B12" s="84"/>
+      <c r="C12" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="67" t="s">
+      <c r="D12" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="67" t="s">
+      <c r="E12" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="68" t="s">
+      <c r="F12" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="67" t="s">
+      <c r="G12" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="67" t="s">
+      <c r="H12" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="I12" s="67" t="s">
+      <c r="I12" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="67" t="s">
+      <c r="J12" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="65" t="s">
+      <c r="K12" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="L12" s="65" t="s">
+      <c r="L12" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="M12" s="70" t="s">
+      <c r="M12" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="N12" s="71"/>
-      <c r="O12" s="71"/>
-      <c r="P12" s="71"/>
-      <c r="Q12" s="71"/>
-      <c r="R12" s="71"/>
-      <c r="S12" s="72"/>
-      <c r="T12" s="70" t="s">
+      <c r="N12" s="74"/>
+      <c r="O12" s="74"/>
+      <c r="P12" s="74"/>
+      <c r="Q12" s="74"/>
+      <c r="R12" s="74"/>
+      <c r="S12" s="75"/>
+      <c r="T12" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="U12" s="71"/>
-      <c r="V12" s="71"/>
-      <c r="W12" s="71"/>
-      <c r="X12" s="72"/>
-      <c r="Y12" s="70" t="s">
+      <c r="U12" s="74"/>
+      <c r="V12" s="74"/>
+      <c r="W12" s="74"/>
+      <c r="X12" s="75"/>
+      <c r="Y12" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="Z12" s="71"/>
-      <c r="AA12" s="71"/>
-      <c r="AB12" s="72"/>
-      <c r="AC12" s="75"/>
+      <c r="Z12" s="74"/>
+      <c r="AA12" s="74"/>
+      <c r="AB12" s="75"/>
+      <c r="AC12" s="80"/>
       <c r="AD12" s="18" t="s">
         <v>75</v>
       </c>
       <c r="AE12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="AF12" s="64"/>
+      <c r="AF12" s="84"/>
     </row>
     <row r="13" spans="1:39" s="20" customFormat="1" ht="124.5" customHeight="1">
       <c r="A13" s="18" t="s">
@@ -1665,16 +1663,16 @@
       <c r="B13" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
       <c r="M13" s="21" t="s">
         <v>28</v>
       </c>
@@ -1723,14 +1721,14 @@
       <c r="AB13" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="AC13" s="76"/>
+      <c r="AC13" s="81"/>
       <c r="AD13" s="21" t="s">
         <v>44</v>
       </c>
       <c r="AE13" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="AF13" s="64"/>
+      <c r="AF13" s="84"/>
     </row>
     <row r="14" spans="1:39" s="20" customFormat="1" ht="20.25" customHeight="1">
       <c r="A14" s="22"/>
@@ -4122,43 +4120,43 @@
       <c r="D85" s="27"/>
       <c r="E85" s="27"/>
       <c r="F85" s="27"/>
-      <c r="H85" s="79" t="s">
+      <c r="H85" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="I85" s="80"/>
-      <c r="J85" s="80"/>
-      <c r="K85" s="80"/>
-      <c r="L85" s="60"/>
-      <c r="M85" s="61"/>
-      <c r="N85" s="62"/>
-      <c r="O85" s="63"/>
-      <c r="P85" s="63"/>
+      <c r="I85" s="52"/>
+      <c r="J85" s="52"/>
+      <c r="K85" s="52"/>
+      <c r="L85" s="53"/>
+      <c r="M85" s="54"/>
+      <c r="N85" s="55"/>
+      <c r="O85" s="56"/>
+      <c r="P85" s="56"/>
       <c r="Q85" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R85" s="30"/>
-      <c r="S85" s="94" t="s">
+      <c r="S85" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="T85" s="95"/>
-      <c r="U85" s="95"/>
-      <c r="V85" s="95"/>
-      <c r="W85" s="95"/>
-      <c r="X85" s="96"/>
-      <c r="Y85" s="94" t="s">
+      <c r="T85" s="58"/>
+      <c r="U85" s="58"/>
+      <c r="V85" s="58"/>
+      <c r="W85" s="58"/>
+      <c r="X85" s="59"/>
+      <c r="Y85" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="Z85" s="95"/>
-      <c r="AA85" s="96"/>
-      <c r="AB85" s="93" t="s">
+      <c r="Z85" s="58"/>
+      <c r="AA85" s="59"/>
+      <c r="AB85" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="AC85" s="93"/>
-      <c r="AD85" s="93"/>
-      <c r="AE85" s="77" t="s">
+      <c r="AC85" s="72"/>
+      <c r="AD85" s="72"/>
+      <c r="AE85" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="AF85" s="78"/>
+      <c r="AF85" s="83"/>
     </row>
     <row r="86" spans="1:32" s="28" customFormat="1" ht="17.25" customHeight="1">
       <c r="A86" s="26"/>
@@ -4168,165 +4166,169 @@
       <c r="E86" s="27"/>
       <c r="F86" s="27"/>
       <c r="G86" s="32"/>
-      <c r="H86" s="79" t="s">
+      <c r="H86" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="I86" s="80"/>
-      <c r="J86" s="80"/>
-      <c r="K86" s="80"/>
-      <c r="L86" s="60"/>
-      <c r="M86" s="61"/>
-      <c r="N86" s="62"/>
-      <c r="O86" s="63"/>
-      <c r="P86" s="63"/>
+      <c r="I86" s="52"/>
+      <c r="J86" s="52"/>
+      <c r="K86" s="52"/>
+      <c r="L86" s="53"/>
+      <c r="M86" s="54"/>
+      <c r="N86" s="55"/>
+      <c r="O86" s="56"/>
+      <c r="P86" s="56"/>
       <c r="Q86" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R86" s="30"/>
-      <c r="S86" s="81" t="s">
+      <c r="S86" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="T86" s="82"/>
-      <c r="U86" s="82"/>
-      <c r="V86" s="82"/>
-      <c r="W86" s="82"/>
-      <c r="X86" s="83"/>
-      <c r="Y86" s="87"/>
-      <c r="Z86" s="88"/>
-      <c r="AA86" s="89"/>
-      <c r="AB86" s="93"/>
-      <c r="AC86" s="93"/>
-      <c r="AD86" s="93"/>
+      <c r="T86" s="61"/>
+      <c r="U86" s="61"/>
+      <c r="V86" s="61"/>
+      <c r="W86" s="61"/>
+      <c r="X86" s="62"/>
+      <c r="Y86" s="66"/>
+      <c r="Z86" s="67"/>
+      <c r="AA86" s="68"/>
+      <c r="AB86" s="72"/>
+      <c r="AC86" s="72"/>
+      <c r="AD86" s="72"/>
       <c r="AE86" s="33"/>
       <c r="AF86" s="34"/>
     </row>
     <row r="87" spans="1:32" s="28" customFormat="1" ht="17.25" customHeight="1">
-      <c r="H87" s="79" t="s">
+      <c r="H87" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="I87" s="80"/>
-      <c r="J87" s="80"/>
-      <c r="K87" s="80"/>
-      <c r="L87" s="60"/>
-      <c r="M87" s="61"/>
-      <c r="N87" s="62"/>
-      <c r="O87" s="63"/>
-      <c r="P87" s="63"/>
+      <c r="I87" s="52"/>
+      <c r="J87" s="52"/>
+      <c r="K87" s="52"/>
+      <c r="L87" s="53"/>
+      <c r="M87" s="54"/>
+      <c r="N87" s="55"/>
+      <c r="O87" s="56"/>
+      <c r="P87" s="56"/>
       <c r="Q87" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R87" s="30"/>
-      <c r="S87" s="84"/>
-      <c r="T87" s="85"/>
-      <c r="U87" s="85"/>
-      <c r="V87" s="85"/>
-      <c r="W87" s="85"/>
-      <c r="X87" s="86"/>
-      <c r="Y87" s="90"/>
-      <c r="Z87" s="91"/>
-      <c r="AA87" s="92"/>
-      <c r="AB87" s="93"/>
-      <c r="AC87" s="93"/>
-      <c r="AD87" s="93"/>
+      <c r="S87" s="63"/>
+      <c r="T87" s="64"/>
+      <c r="U87" s="64"/>
+      <c r="V87" s="64"/>
+      <c r="W87" s="64"/>
+      <c r="X87" s="65"/>
+      <c r="Y87" s="69"/>
+      <c r="Z87" s="70"/>
+      <c r="AA87" s="71"/>
+      <c r="AB87" s="72"/>
+      <c r="AC87" s="72"/>
+      <c r="AD87" s="72"/>
     </row>
     <row r="88" spans="1:32" s="28" customFormat="1" ht="17.25" customHeight="1">
       <c r="A88" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="H88" s="79" t="s">
+      <c r="H88" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="I88" s="80"/>
-      <c r="J88" s="80"/>
-      <c r="K88" s="80"/>
-      <c r="L88" s="60"/>
-      <c r="M88" s="61"/>
-      <c r="N88" s="62"/>
-      <c r="O88" s="63"/>
-      <c r="P88" s="63"/>
+      <c r="I88" s="52"/>
+      <c r="J88" s="52"/>
+      <c r="K88" s="52"/>
+      <c r="L88" s="53"/>
+      <c r="M88" s="54"/>
+      <c r="N88" s="55"/>
+      <c r="O88" s="56"/>
+      <c r="P88" s="56"/>
       <c r="Q88" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R88" s="30"/>
-      <c r="S88" s="81" t="s">
+      <c r="S88" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="T88" s="82"/>
-      <c r="U88" s="82"/>
-      <c r="V88" s="82"/>
-      <c r="W88" s="82"/>
-      <c r="X88" s="83"/>
-      <c r="Y88" s="87"/>
-      <c r="Z88" s="88"/>
-      <c r="AA88" s="89"/>
-      <c r="AB88" s="93"/>
-      <c r="AC88" s="93"/>
-      <c r="AD88" s="93"/>
+      <c r="T88" s="61"/>
+      <c r="U88" s="61"/>
+      <c r="V88" s="61"/>
+      <c r="W88" s="61"/>
+      <c r="X88" s="62"/>
+      <c r="Y88" s="66"/>
+      <c r="Z88" s="67"/>
+      <c r="AA88" s="68"/>
+      <c r="AB88" s="72"/>
+      <c r="AC88" s="72"/>
+      <c r="AD88" s="72"/>
     </row>
     <row r="89" spans="1:32" s="28" customFormat="1" ht="17.25" customHeight="1">
       <c r="A89" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="H89" s="79" t="s">
+      <c r="H89" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="I89" s="80"/>
-      <c r="J89" s="80"/>
-      <c r="K89" s="80"/>
-      <c r="L89" s="60"/>
-      <c r="M89" s="61"/>
-      <c r="N89" s="62"/>
-      <c r="O89" s="63"/>
-      <c r="P89" s="63"/>
+      <c r="I89" s="52"/>
+      <c r="J89" s="52"/>
+      <c r="K89" s="52"/>
+      <c r="L89" s="53"/>
+      <c r="M89" s="54"/>
+      <c r="N89" s="55"/>
+      <c r="O89" s="56"/>
+      <c r="P89" s="56"/>
       <c r="Q89" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R89" s="30"/>
-      <c r="S89" s="84"/>
-      <c r="T89" s="85"/>
-      <c r="U89" s="85"/>
-      <c r="V89" s="85"/>
-      <c r="W89" s="85"/>
-      <c r="X89" s="86"/>
-      <c r="Y89" s="90"/>
-      <c r="Z89" s="91"/>
-      <c r="AA89" s="92"/>
-      <c r="AB89" s="93"/>
-      <c r="AC89" s="93"/>
-      <c r="AD89" s="93"/>
+      <c r="S89" s="63"/>
+      <c r="T89" s="64"/>
+      <c r="U89" s="64"/>
+      <c r="V89" s="64"/>
+      <c r="W89" s="64"/>
+      <c r="X89" s="65"/>
+      <c r="Y89" s="69"/>
+      <c r="Z89" s="70"/>
+      <c r="AA89" s="71"/>
+      <c r="AB89" s="72"/>
+      <c r="AC89" s="72"/>
+      <c r="AD89" s="72"/>
     </row>
     <row r="90" spans="1:32" s="28" customFormat="1" ht="14.25"/>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AB6:AD6"/>
+    <mergeCell ref="AE9:AF9"/>
     <mergeCell ref="AB8:AD8"/>
     <mergeCell ref="AB9:AD9"/>
-    <mergeCell ref="A3:AF3"/>
-    <mergeCell ref="A4:AF4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="H89:K89"/>
-    <mergeCell ref="L89:M89"/>
-    <mergeCell ref="N89:P89"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="L88:M88"/>
-    <mergeCell ref="S85:X85"/>
-    <mergeCell ref="N88:P88"/>
-    <mergeCell ref="S88:X89"/>
-    <mergeCell ref="Y88:AA89"/>
-    <mergeCell ref="AB88:AD89"/>
+    <mergeCell ref="AB7:AD7"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="P7:Q8"/>
+    <mergeCell ref="R7:S8"/>
+    <mergeCell ref="T7:U8"/>
+    <mergeCell ref="V7:W8"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="L85:M85"/>
+    <mergeCell ref="N85:P85"/>
+    <mergeCell ref="AF11:AF13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="Y12:AB12"/>
+    <mergeCell ref="T12:X12"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
     <mergeCell ref="M12:S12"/>
     <mergeCell ref="M11:AB11"/>
     <mergeCell ref="AC11:AC13"/>
@@ -4343,29 +4345,21 @@
     <mergeCell ref="AB85:AD85"/>
     <mergeCell ref="Y85:AA85"/>
     <mergeCell ref="H85:K85"/>
-    <mergeCell ref="L85:M85"/>
-    <mergeCell ref="N85:P85"/>
-    <mergeCell ref="AF11:AF13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="Y12:AB12"/>
-    <mergeCell ref="T12:X12"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="S85:X85"/>
+    <mergeCell ref="N88:P88"/>
+    <mergeCell ref="S88:X89"/>
+    <mergeCell ref="Y88:AA89"/>
+    <mergeCell ref="AB88:AD89"/>
+    <mergeCell ref="H89:K89"/>
+    <mergeCell ref="L89:M89"/>
+    <mergeCell ref="N89:P89"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="L88:M88"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="N6:O6"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="D8:H8"/>
     <mergeCell ref="J8:K8"/>
@@ -4373,16 +4367,20 @@
     <mergeCell ref="A6:C7"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="N7:O8"/>
-    <mergeCell ref="AE9:AF9"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AB6:AD6"/>
+    <mergeCell ref="A3:AF3"/>
+    <mergeCell ref="A4:AF4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="T6:U6"/>
     <mergeCell ref="V6:W6"/>
     <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AB7:AD7"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="P7:Q8"/>
-    <mergeCell ref="R7:S8"/>
-    <mergeCell ref="T7:U8"/>
-    <mergeCell ref="V7:W8"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A85:K89 AC8:AD9 A3:AF4 J6:K9 A11:E13 G11:H11 J11:K11 F12:AB13 M11:AB11 Q85:AF89 AC11:AF13 A1:AE2 A8:C9 B5:C5 A5:A6 AB6:AB9 AC6:AD6 N6:N7 P6:W7 O6" xr:uid="{01C90C96-D563-415B-B968-F3ADF92B0BE3}">
@@ -4420,10 +4418,10 @@
         <v>0</v>
       </c>
       <c r="AD1" s="3"/>
-      <c r="AE1" s="97" t="s">
+      <c r="AE1" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="AF1" s="97"/>
+      <c r="AF1" s="42"/>
       <c r="AI1" s="4"/>
       <c r="AJ1" s="4"/>
       <c r="AK1" s="4"/>
@@ -4434,222 +4432,222 @@
       <c r="A2" s="5"/>
       <c r="AC2" s="6"/>
       <c r="AD2" s="6"/>
-      <c r="AE2" s="104" t="s">
+      <c r="AE2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="AF2" s="104"/>
+      <c r="AF2" s="39"/>
     </row>
     <row r="3" spans="1:39" s="7" customFormat="1" ht="26.25">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="98"/>
-      <c r="R3" s="98"/>
-      <c r="S3" s="98"/>
-      <c r="T3" s="98"/>
-      <c r="U3" s="98"/>
-      <c r="V3" s="98"/>
-      <c r="W3" s="98"/>
-      <c r="X3" s="98"/>
-      <c r="Y3" s="98"/>
-      <c r="Z3" s="98"/>
-      <c r="AA3" s="98"/>
-      <c r="AB3" s="98"/>
-      <c r="AC3" s="98"/>
-      <c r="AD3" s="98"/>
-      <c r="AE3" s="98"/>
-      <c r="AF3" s="98"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="47"/>
+      <c r="Z3" s="47"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="47"/>
+      <c r="AC3" s="47"/>
+      <c r="AD3" s="47"/>
+      <c r="AE3" s="47"/>
+      <c r="AF3" s="47"/>
     </row>
     <row r="4" spans="1:39" s="8" customFormat="1" ht="19.5">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
-      <c r="N4" s="99"/>
-      <c r="O4" s="99"/>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="99"/>
-      <c r="V4" s="99"/>
-      <c r="W4" s="99"/>
-      <c r="X4" s="99"/>
-      <c r="Y4" s="99"/>
-      <c r="Z4" s="99"/>
-      <c r="AA4" s="99"/>
-      <c r="AB4" s="99"/>
-      <c r="AC4" s="99"/>
-      <c r="AD4" s="99"/>
-      <c r="AE4" s="99"/>
-      <c r="AF4" s="99"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="48"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="48"/>
+      <c r="AD4" s="48"/>
+      <c r="AE4" s="48"/>
+      <c r="AF4" s="48"/>
     </row>
     <row r="5" spans="1:39" s="10" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="AC5" s="100"/>
-      <c r="AD5" s="100"/>
-      <c r="AE5" s="101"/>
-      <c r="AF5" s="101"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="49"/>
+      <c r="AE5" s="50"/>
+      <c r="AF5" s="50"/>
     </row>
     <row r="6" spans="1:39" s="10" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="J6" s="53" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="93"/>
+      <c r="H6" s="93"/>
+      <c r="J6" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="53"/>
+      <c r="K6" s="46"/>
       <c r="L6" s="11"/>
-      <c r="N6" s="44" t="s">
+      <c r="N6" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="45"/>
-      <c r="P6" s="44" t="s">
+      <c r="O6" s="41"/>
+      <c r="P6" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="44" t="s">
+      <c r="Q6" s="41"/>
+      <c r="R6" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="45"/>
-      <c r="T6" s="44" t="s">
+      <c r="S6" s="41"/>
+      <c r="T6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="U6" s="45"/>
-      <c r="V6" s="44" t="s">
+      <c r="U6" s="41"/>
+      <c r="V6" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="W6" s="45"/>
-      <c r="AB6" s="48" t="s">
+      <c r="W6" s="41"/>
+      <c r="AB6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="AC6" s="48"/>
-      <c r="AD6" s="49"/>
-      <c r="AE6" s="46"/>
-      <c r="AF6" s="47"/>
+      <c r="AC6" s="43"/>
+      <c r="AD6" s="44"/>
+      <c r="AE6" s="98"/>
+      <c r="AF6" s="99"/>
     </row>
     <row r="7" spans="1:39" s="10" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="J7" s="53" t="s">
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="J7" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="49"/>
+      <c r="K7" s="44"/>
       <c r="L7" s="11"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="40"/>
-      <c r="V7" s="39"/>
-      <c r="W7" s="40"/>
-      <c r="AB7" s="48" t="s">
+      <c r="N7" s="94"/>
+      <c r="O7" s="95"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="95"/>
+      <c r="R7" s="94"/>
+      <c r="S7" s="95"/>
+      <c r="T7" s="94"/>
+      <c r="U7" s="95"/>
+      <c r="V7" s="94"/>
+      <c r="W7" s="95"/>
+      <c r="AB7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="AC7" s="48"/>
-      <c r="AD7" s="49"/>
-      <c r="AE7" s="50"/>
-      <c r="AF7" s="51"/>
+      <c r="AC7" s="43"/>
+      <c r="AD7" s="44"/>
+      <c r="AE7" s="100"/>
+      <c r="AF7" s="101"/>
     </row>
     <row r="8" spans="1:39" s="10" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="J8" s="53" t="s">
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="J8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="53"/>
+      <c r="K8" s="46"/>
       <c r="L8" s="11"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="41"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="41"/>
-      <c r="U8" s="42"/>
-      <c r="V8" s="41"/>
-      <c r="W8" s="42"/>
-      <c r="AB8" s="48" t="s">
+      <c r="N8" s="96"/>
+      <c r="O8" s="97"/>
+      <c r="P8" s="96"/>
+      <c r="Q8" s="97"/>
+      <c r="R8" s="96"/>
+      <c r="S8" s="97"/>
+      <c r="T8" s="96"/>
+      <c r="U8" s="97"/>
+      <c r="V8" s="96"/>
+      <c r="W8" s="97"/>
+      <c r="AB8" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="AC8" s="48"/>
-      <c r="AD8" s="49"/>
-      <c r="AE8" s="102"/>
-      <c r="AF8" s="103"/>
+      <c r="AC8" s="43"/>
+      <c r="AD8" s="44"/>
+      <c r="AE8" s="103"/>
+      <c r="AF8" s="104"/>
     </row>
     <row r="9" spans="1:39" s="10" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
       <c r="L9" s="37"/>
       <c r="M9" s="36"/>
       <c r="N9" s="38"/>
@@ -4666,61 +4664,61 @@
       <c r="Y9" s="36"/>
       <c r="Z9" s="36"/>
       <c r="AA9" s="36"/>
-      <c r="AB9" s="53"/>
-      <c r="AC9" s="53"/>
-      <c r="AD9" s="53"/>
-      <c r="AE9" s="43"/>
-      <c r="AF9" s="43"/>
+      <c r="AB9" s="46"/>
+      <c r="AC9" s="46"/>
+      <c r="AD9" s="46"/>
+      <c r="AE9" s="102"/>
+      <c r="AF9" s="102"/>
     </row>
     <row r="10" spans="1:39" s="10" customFormat="1" ht="6" customHeight="1">
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="90"/>
+      <c r="L10" s="90"/>
     </row>
     <row r="11" spans="1:39" s="31" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="58" t="s">
+      <c r="B11" s="78"/>
+      <c r="C11" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="59"/>
+      <c r="H11" s="92"/>
       <c r="I11" s="13"/>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="59"/>
+      <c r="K11" s="92"/>
       <c r="L11" s="13"/>
-      <c r="M11" s="56" t="s">
+      <c r="M11" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="73"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
-      <c r="R11" s="73"/>
-      <c r="S11" s="73"/>
-      <c r="T11" s="73"/>
-      <c r="U11" s="73"/>
-      <c r="V11" s="73"/>
-      <c r="W11" s="73"/>
-      <c r="X11" s="73"/>
-      <c r="Y11" s="73"/>
-      <c r="Z11" s="73"/>
-      <c r="AA11" s="73"/>
-      <c r="AB11" s="57"/>
-      <c r="AC11" s="74" t="s">
+      <c r="N11" s="77"/>
+      <c r="O11" s="77"/>
+      <c r="P11" s="77"/>
+      <c r="Q11" s="77"/>
+      <c r="R11" s="77"/>
+      <c r="S11" s="77"/>
+      <c r="T11" s="77"/>
+      <c r="U11" s="77"/>
+      <c r="V11" s="77"/>
+      <c r="W11" s="77"/>
+      <c r="X11" s="77"/>
+      <c r="Y11" s="77"/>
+      <c r="Z11" s="77"/>
+      <c r="AA11" s="77"/>
+      <c r="AB11" s="78"/>
+      <c r="AC11" s="79" t="s">
         <v>19</v>
       </c>
       <c r="AD11" s="16" t="s">
@@ -4729,75 +4727,75 @@
       <c r="AE11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="AF11" s="64" t="s">
+      <c r="AF11" s="84" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:39" s="20" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="65" t="s">
+      <c r="B12" s="84"/>
+      <c r="C12" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="67" t="s">
+      <c r="D12" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="67" t="s">
+      <c r="E12" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="68" t="s">
+      <c r="F12" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="67" t="s">
+      <c r="G12" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="67" t="s">
+      <c r="H12" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="I12" s="67" t="s">
+      <c r="I12" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="67" t="s">
+      <c r="J12" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="65" t="s">
+      <c r="K12" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="L12" s="65" t="s">
+      <c r="L12" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="M12" s="70" t="s">
+      <c r="M12" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="N12" s="71"/>
-      <c r="O12" s="71"/>
-      <c r="P12" s="71"/>
-      <c r="Q12" s="71"/>
-      <c r="R12" s="71"/>
-      <c r="S12" s="72"/>
-      <c r="T12" s="70" t="s">
+      <c r="N12" s="74"/>
+      <c r="O12" s="74"/>
+      <c r="P12" s="74"/>
+      <c r="Q12" s="74"/>
+      <c r="R12" s="74"/>
+      <c r="S12" s="75"/>
+      <c r="T12" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="U12" s="71"/>
-      <c r="V12" s="71"/>
-      <c r="W12" s="71"/>
-      <c r="X12" s="72"/>
-      <c r="Y12" s="70" t="s">
+      <c r="U12" s="74"/>
+      <c r="V12" s="74"/>
+      <c r="W12" s="74"/>
+      <c r="X12" s="75"/>
+      <c r="Y12" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="Z12" s="71"/>
-      <c r="AA12" s="71"/>
-      <c r="AB12" s="72"/>
-      <c r="AC12" s="75"/>
+      <c r="Z12" s="74"/>
+      <c r="AA12" s="74"/>
+      <c r="AB12" s="75"/>
+      <c r="AC12" s="80"/>
       <c r="AD12" s="18" t="s">
         <v>75</v>
       </c>
       <c r="AE12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="AF12" s="64"/>
+      <c r="AF12" s="84"/>
     </row>
     <row r="13" spans="1:39" s="20" customFormat="1" ht="124.5" customHeight="1">
       <c r="A13" s="18" t="s">
@@ -4806,16 +4804,16 @@
       <c r="B13" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
       <c r="M13" s="21" t="s">
         <v>28</v>
       </c>
@@ -4864,14 +4862,14 @@
       <c r="AB13" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="AC13" s="76"/>
+      <c r="AC13" s="81"/>
       <c r="AD13" s="21" t="s">
         <v>44</v>
       </c>
       <c r="AE13" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="AF13" s="64"/>
+      <c r="AF13" s="84"/>
     </row>
     <row r="14" spans="1:39" s="20" customFormat="1" ht="20.25" customHeight="1">
       <c r="A14" s="22"/>
@@ -7263,43 +7261,43 @@
       <c r="D85" s="27"/>
       <c r="E85" s="27"/>
       <c r="F85" s="27"/>
-      <c r="H85" s="79" t="s">
+      <c r="H85" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="I85" s="80"/>
-      <c r="J85" s="80"/>
-      <c r="K85" s="80"/>
-      <c r="L85" s="60"/>
-      <c r="M85" s="61"/>
-      <c r="N85" s="62"/>
-      <c r="O85" s="63"/>
-      <c r="P85" s="63"/>
+      <c r="I85" s="52"/>
+      <c r="J85" s="52"/>
+      <c r="K85" s="52"/>
+      <c r="L85" s="53"/>
+      <c r="M85" s="54"/>
+      <c r="N85" s="55"/>
+      <c r="O85" s="56"/>
+      <c r="P85" s="56"/>
       <c r="Q85" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R85" s="30"/>
-      <c r="S85" s="94" t="s">
+      <c r="S85" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="T85" s="95"/>
-      <c r="U85" s="95"/>
-      <c r="V85" s="95"/>
-      <c r="W85" s="95"/>
-      <c r="X85" s="96"/>
-      <c r="Y85" s="94" t="s">
+      <c r="T85" s="58"/>
+      <c r="U85" s="58"/>
+      <c r="V85" s="58"/>
+      <c r="W85" s="58"/>
+      <c r="X85" s="59"/>
+      <c r="Y85" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="Z85" s="95"/>
-      <c r="AA85" s="96"/>
-      <c r="AB85" s="93" t="s">
+      <c r="Z85" s="58"/>
+      <c r="AA85" s="59"/>
+      <c r="AB85" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="AC85" s="93"/>
-      <c r="AD85" s="93"/>
-      <c r="AE85" s="77" t="s">
+      <c r="AC85" s="72"/>
+      <c r="AD85" s="72"/>
+      <c r="AE85" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="AF85" s="78"/>
+      <c r="AF85" s="83"/>
     </row>
     <row r="86" spans="1:32" s="28" customFormat="1" ht="17.25" customHeight="1">
       <c r="A86" s="26"/>
@@ -7309,167 +7307,176 @@
       <c r="E86" s="27"/>
       <c r="F86" s="27"/>
       <c r="G86" s="32"/>
-      <c r="H86" s="79" t="s">
+      <c r="H86" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="I86" s="80"/>
-      <c r="J86" s="80"/>
-      <c r="K86" s="80"/>
-      <c r="L86" s="60"/>
-      <c r="M86" s="61"/>
-      <c r="N86" s="62"/>
-      <c r="O86" s="63"/>
-      <c r="P86" s="63"/>
+      <c r="I86" s="52"/>
+      <c r="J86" s="52"/>
+      <c r="K86" s="52"/>
+      <c r="L86" s="53"/>
+      <c r="M86" s="54"/>
+      <c r="N86" s="55"/>
+      <c r="O86" s="56"/>
+      <c r="P86" s="56"/>
       <c r="Q86" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R86" s="30"/>
-      <c r="S86" s="81" t="s">
+      <c r="S86" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="T86" s="82"/>
-      <c r="U86" s="82"/>
-      <c r="V86" s="82"/>
-      <c r="W86" s="82"/>
-      <c r="X86" s="83"/>
-      <c r="Y86" s="87"/>
-      <c r="Z86" s="88"/>
-      <c r="AA86" s="89"/>
-      <c r="AB86" s="93"/>
-      <c r="AC86" s="93"/>
-      <c r="AD86" s="93"/>
+      <c r="T86" s="61"/>
+      <c r="U86" s="61"/>
+      <c r="V86" s="61"/>
+      <c r="W86" s="61"/>
+      <c r="X86" s="62"/>
+      <c r="Y86" s="66"/>
+      <c r="Z86" s="67"/>
+      <c r="AA86" s="68"/>
+      <c r="AB86" s="72"/>
+      <c r="AC86" s="72"/>
+      <c r="AD86" s="72"/>
       <c r="AE86" s="33"/>
       <c r="AF86" s="34"/>
     </row>
     <row r="87" spans="1:32" s="28" customFormat="1" ht="17.25" customHeight="1">
-      <c r="H87" s="79" t="s">
+      <c r="H87" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="I87" s="80"/>
-      <c r="J87" s="80"/>
-      <c r="K87" s="80"/>
-      <c r="L87" s="60"/>
-      <c r="M87" s="61"/>
-      <c r="N87" s="62"/>
-      <c r="O87" s="63"/>
-      <c r="P87" s="63"/>
+      <c r="I87" s="52"/>
+      <c r="J87" s="52"/>
+      <c r="K87" s="52"/>
+      <c r="L87" s="53"/>
+      <c r="M87" s="54"/>
+      <c r="N87" s="55"/>
+      <c r="O87" s="56"/>
+      <c r="P87" s="56"/>
       <c r="Q87" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R87" s="30"/>
-      <c r="S87" s="84"/>
-      <c r="T87" s="85"/>
-      <c r="U87" s="85"/>
-      <c r="V87" s="85"/>
-      <c r="W87" s="85"/>
-      <c r="X87" s="86"/>
-      <c r="Y87" s="90"/>
-      <c r="Z87" s="91"/>
-      <c r="AA87" s="92"/>
-      <c r="AB87" s="93"/>
-      <c r="AC87" s="93"/>
-      <c r="AD87" s="93"/>
+      <c r="S87" s="63"/>
+      <c r="T87" s="64"/>
+      <c r="U87" s="64"/>
+      <c r="V87" s="64"/>
+      <c r="W87" s="64"/>
+      <c r="X87" s="65"/>
+      <c r="Y87" s="69"/>
+      <c r="Z87" s="70"/>
+      <c r="AA87" s="71"/>
+      <c r="AB87" s="72"/>
+      <c r="AC87" s="72"/>
+      <c r="AD87" s="72"/>
     </row>
     <row r="88" spans="1:32" s="28" customFormat="1" ht="17.25" customHeight="1">
       <c r="A88" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="H88" s="79" t="s">
+      <c r="H88" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="I88" s="80"/>
-      <c r="J88" s="80"/>
-      <c r="K88" s="80"/>
-      <c r="L88" s="60"/>
-      <c r="M88" s="61"/>
-      <c r="N88" s="62"/>
-      <c r="O88" s="63"/>
-      <c r="P88" s="63"/>
+      <c r="I88" s="52"/>
+      <c r="J88" s="52"/>
+      <c r="K88" s="52"/>
+      <c r="L88" s="53"/>
+      <c r="M88" s="54"/>
+      <c r="N88" s="55"/>
+      <c r="O88" s="56"/>
+      <c r="P88" s="56"/>
       <c r="Q88" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R88" s="30"/>
-      <c r="S88" s="81" t="s">
+      <c r="S88" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="T88" s="82"/>
-      <c r="U88" s="82"/>
-      <c r="V88" s="82"/>
-      <c r="W88" s="82"/>
-      <c r="X88" s="83"/>
-      <c r="Y88" s="87"/>
-      <c r="Z88" s="88"/>
-      <c r="AA88" s="89"/>
-      <c r="AB88" s="93"/>
-      <c r="AC88" s="93"/>
-      <c r="AD88" s="93"/>
+      <c r="T88" s="61"/>
+      <c r="U88" s="61"/>
+      <c r="V88" s="61"/>
+      <c r="W88" s="61"/>
+      <c r="X88" s="62"/>
+      <c r="Y88" s="66"/>
+      <c r="Z88" s="67"/>
+      <c r="AA88" s="68"/>
+      <c r="AB88" s="72"/>
+      <c r="AC88" s="72"/>
+      <c r="AD88" s="72"/>
     </row>
     <row r="89" spans="1:32" s="28" customFormat="1" ht="17.25" customHeight="1">
       <c r="A89" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="H89" s="79" t="s">
+      <c r="H89" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="I89" s="80"/>
-      <c r="J89" s="80"/>
-      <c r="K89" s="80"/>
-      <c r="L89" s="60"/>
-      <c r="M89" s="61"/>
-      <c r="N89" s="62"/>
-      <c r="O89" s="63"/>
-      <c r="P89" s="63"/>
+      <c r="I89" s="52"/>
+      <c r="J89" s="52"/>
+      <c r="K89" s="52"/>
+      <c r="L89" s="53"/>
+      <c r="M89" s="54"/>
+      <c r="N89" s="55"/>
+      <c r="O89" s="56"/>
+      <c r="P89" s="56"/>
       <c r="Q89" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R89" s="30"/>
-      <c r="S89" s="84"/>
-      <c r="T89" s="85"/>
-      <c r="U89" s="85"/>
-      <c r="V89" s="85"/>
-      <c r="W89" s="85"/>
-      <c r="X89" s="86"/>
-      <c r="Y89" s="90"/>
-      <c r="Z89" s="91"/>
-      <c r="AA89" s="92"/>
-      <c r="AB89" s="93"/>
-      <c r="AC89" s="93"/>
-      <c r="AD89" s="93"/>
+      <c r="S89" s="63"/>
+      <c r="T89" s="64"/>
+      <c r="U89" s="64"/>
+      <c r="V89" s="64"/>
+      <c r="W89" s="64"/>
+      <c r="X89" s="65"/>
+      <c r="Y89" s="69"/>
+      <c r="Z89" s="70"/>
+      <c r="AA89" s="71"/>
+      <c r="AB89" s="72"/>
+      <c r="AC89" s="72"/>
+      <c r="AD89" s="72"/>
     </row>
     <row r="90" spans="1:32" s="28" customFormat="1" ht="14.25"/>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="AE85:AF85"/>
-    <mergeCell ref="S86:X87"/>
-    <mergeCell ref="Y86:AA87"/>
-    <mergeCell ref="AB86:AD87"/>
-    <mergeCell ref="S88:X89"/>
-    <mergeCell ref="Y88:AA89"/>
-    <mergeCell ref="AB88:AD89"/>
-    <mergeCell ref="Y12:AB12"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="H89:K89"/>
-    <mergeCell ref="L89:M89"/>
-    <mergeCell ref="N89:P89"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="L86:M86"/>
-    <mergeCell ref="N86:P86"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="A3:AF3"/>
+    <mergeCell ref="A4:AF4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="D6:H7"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="AB6:AD6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="N7:O8"/>
+    <mergeCell ref="P7:Q8"/>
+    <mergeCell ref="R7:S8"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="T7:U8"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="M11:AB11"/>
+    <mergeCell ref="V7:W8"/>
+    <mergeCell ref="AB7:AD7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="AB8:AD8"/>
     <mergeCell ref="AC11:AC13"/>
     <mergeCell ref="AB9:AD9"/>
-    <mergeCell ref="AF11:AF13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:S12"/>
-    <mergeCell ref="T12:X12"/>
     <mergeCell ref="AE9:AF9"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
@@ -7486,44 +7493,35 @@
     <mergeCell ref="H85:K85"/>
     <mergeCell ref="L85:M85"/>
     <mergeCell ref="N85:P85"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="T7:U8"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="M11:AB11"/>
-    <mergeCell ref="V7:W8"/>
-    <mergeCell ref="AB7:AD7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="AB8:AD8"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="D6:H7"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="AB6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="N7:O8"/>
-    <mergeCell ref="P7:Q8"/>
-    <mergeCell ref="R7:S8"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="A3:AF3"/>
-    <mergeCell ref="A4:AF4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AF11:AF13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:S12"/>
+    <mergeCell ref="T12:X12"/>
+    <mergeCell ref="Y12:AB12"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="H89:K89"/>
+    <mergeCell ref="L89:M89"/>
+    <mergeCell ref="N89:P89"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="L86:M86"/>
+    <mergeCell ref="N86:P86"/>
+    <mergeCell ref="AE85:AF85"/>
+    <mergeCell ref="S86:X87"/>
+    <mergeCell ref="Y86:AA87"/>
+    <mergeCell ref="AB86:AD87"/>
+    <mergeCell ref="S88:X89"/>
+    <mergeCell ref="Y88:AA89"/>
+    <mergeCell ref="AB88:AD89"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A85:K89 AC8:AD9 A3:AF4 J6:K9 A11:E13 G11:H11 J11:K11 F12:AB13 M11:AB11 Q85:AF89 AC11:AF13 A1:AE2 A8:C9 B5:C5 A5:A6 AB6:AB9 AC6:AD6 N6:N7 P6:W7 O6" xr:uid="{35757C96-C5B8-4DF2-B84A-572DF468C92E}">
@@ -7561,10 +7559,10 @@
         <v>0</v>
       </c>
       <c r="AD1" s="3"/>
-      <c r="AE1" s="97" t="s">
+      <c r="AE1" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="AF1" s="97"/>
+      <c r="AF1" s="42"/>
       <c r="AI1" s="4"/>
       <c r="AJ1" s="4"/>
       <c r="AK1" s="4"/>
@@ -7575,222 +7573,222 @@
       <c r="A2" s="5"/>
       <c r="AC2" s="6"/>
       <c r="AD2" s="6"/>
-      <c r="AE2" s="104" t="s">
+      <c r="AE2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="AF2" s="104"/>
+      <c r="AF2" s="39"/>
     </row>
     <row r="3" spans="1:39" s="7" customFormat="1" ht="26.25">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
-      <c r="L3" s="98"/>
-      <c r="M3" s="98"/>
-      <c r="N3" s="98"/>
-      <c r="O3" s="98"/>
-      <c r="P3" s="98"/>
-      <c r="Q3" s="98"/>
-      <c r="R3" s="98"/>
-      <c r="S3" s="98"/>
-      <c r="T3" s="98"/>
-      <c r="U3" s="98"/>
-      <c r="V3" s="98"/>
-      <c r="W3" s="98"/>
-      <c r="X3" s="98"/>
-      <c r="Y3" s="98"/>
-      <c r="Z3" s="98"/>
-      <c r="AA3" s="98"/>
-      <c r="AB3" s="98"/>
-      <c r="AC3" s="98"/>
-      <c r="AD3" s="98"/>
-      <c r="AE3" s="98"/>
-      <c r="AF3" s="98"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="47"/>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="47"/>
+      <c r="Z3" s="47"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="47"/>
+      <c r="AC3" s="47"/>
+      <c r="AD3" s="47"/>
+      <c r="AE3" s="47"/>
+      <c r="AF3" s="47"/>
     </row>
     <row r="4" spans="1:39" s="8" customFormat="1" ht="19.5">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
-      <c r="N4" s="99"/>
-      <c r="O4" s="99"/>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="99"/>
-      <c r="V4" s="99"/>
-      <c r="W4" s="99"/>
-      <c r="X4" s="99"/>
-      <c r="Y4" s="99"/>
-      <c r="Z4" s="99"/>
-      <c r="AA4" s="99"/>
-      <c r="AB4" s="99"/>
-      <c r="AC4" s="99"/>
-      <c r="AD4" s="99"/>
-      <c r="AE4" s="99"/>
-      <c r="AF4" s="99"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="48"/>
+      <c r="AB4" s="48"/>
+      <c r="AC4" s="48"/>
+      <c r="AD4" s="48"/>
+      <c r="AE4" s="48"/>
+      <c r="AF4" s="48"/>
     </row>
     <row r="5" spans="1:39" s="10" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="AC5" s="100"/>
-      <c r="AD5" s="100"/>
-      <c r="AE5" s="101"/>
-      <c r="AF5" s="101"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="49"/>
+      <c r="AE5" s="50"/>
+      <c r="AF5" s="50"/>
     </row>
     <row r="6" spans="1:39" s="10" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="J6" s="53" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="93"/>
+      <c r="H6" s="93"/>
+      <c r="J6" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="53"/>
+      <c r="K6" s="46"/>
       <c r="L6" s="11"/>
-      <c r="N6" s="44" t="s">
+      <c r="N6" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="45"/>
-      <c r="P6" s="44" t="s">
+      <c r="O6" s="41"/>
+      <c r="P6" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="44" t="s">
+      <c r="Q6" s="41"/>
+      <c r="R6" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="S6" s="45"/>
-      <c r="T6" s="44" t="s">
+      <c r="S6" s="41"/>
+      <c r="T6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="U6" s="45"/>
-      <c r="V6" s="44" t="s">
+      <c r="U6" s="41"/>
+      <c r="V6" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="W6" s="45"/>
-      <c r="AB6" s="48" t="s">
+      <c r="W6" s="41"/>
+      <c r="AB6" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="AC6" s="48"/>
-      <c r="AD6" s="49"/>
-      <c r="AE6" s="46"/>
-      <c r="AF6" s="47"/>
+      <c r="AC6" s="43"/>
+      <c r="AD6" s="44"/>
+      <c r="AE6" s="98"/>
+      <c r="AF6" s="99"/>
     </row>
     <row r="7" spans="1:39" s="10" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="J7" s="53" t="s">
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="J7" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="49"/>
+      <c r="K7" s="44"/>
       <c r="L7" s="11"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="40"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="40"/>
-      <c r="V7" s="39"/>
-      <c r="W7" s="40"/>
-      <c r="AB7" s="48" t="s">
+      <c r="N7" s="94"/>
+      <c r="O7" s="95"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="95"/>
+      <c r="R7" s="94"/>
+      <c r="S7" s="95"/>
+      <c r="T7" s="94"/>
+      <c r="U7" s="95"/>
+      <c r="V7" s="94"/>
+      <c r="W7" s="95"/>
+      <c r="AB7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="AC7" s="48"/>
-      <c r="AD7" s="49"/>
-      <c r="AE7" s="50"/>
-      <c r="AF7" s="51"/>
+      <c r="AC7" s="43"/>
+      <c r="AD7" s="44"/>
+      <c r="AE7" s="100"/>
+      <c r="AF7" s="101"/>
     </row>
     <row r="8" spans="1:39" s="10" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="J8" s="53" t="s">
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="J8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="53"/>
+      <c r="K8" s="46"/>
       <c r="L8" s="11"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="41"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="41"/>
-      <c r="U8" s="42"/>
-      <c r="V8" s="41"/>
-      <c r="W8" s="42"/>
-      <c r="AB8" s="48" t="s">
+      <c r="N8" s="96"/>
+      <c r="O8" s="97"/>
+      <c r="P8" s="96"/>
+      <c r="Q8" s="97"/>
+      <c r="R8" s="96"/>
+      <c r="S8" s="97"/>
+      <c r="T8" s="96"/>
+      <c r="U8" s="97"/>
+      <c r="V8" s="96"/>
+      <c r="W8" s="97"/>
+      <c r="AB8" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="AC8" s="48"/>
-      <c r="AD8" s="49"/>
-      <c r="AE8" s="102"/>
-      <c r="AF8" s="103"/>
+      <c r="AC8" s="43"/>
+      <c r="AD8" s="44"/>
+      <c r="AE8" s="103"/>
+      <c r="AF8" s="104"/>
     </row>
     <row r="9" spans="1:39" s="10" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
       <c r="L9" s="37"/>
       <c r="M9" s="36"/>
       <c r="N9" s="38"/>
@@ -7807,61 +7805,61 @@
       <c r="Y9" s="36"/>
       <c r="Z9" s="36"/>
       <c r="AA9" s="36"/>
-      <c r="AB9" s="53"/>
-      <c r="AC9" s="53"/>
-      <c r="AD9" s="53"/>
-      <c r="AE9" s="43"/>
-      <c r="AF9" s="43"/>
+      <c r="AB9" s="46"/>
+      <c r="AC9" s="46"/>
+      <c r="AD9" s="46"/>
+      <c r="AE9" s="102"/>
+      <c r="AF9" s="102"/>
     </row>
     <row r="10" spans="1:39" s="10" customFormat="1" ht="6" customHeight="1">
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="90"/>
+      <c r="L10" s="90"/>
     </row>
     <row r="11" spans="1:39" s="31" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="58" t="s">
+      <c r="B11" s="78"/>
+      <c r="C11" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="H11" s="59"/>
+      <c r="H11" s="92"/>
       <c r="I11" s="13"/>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="59"/>
+      <c r="K11" s="92"/>
       <c r="L11" s="13"/>
-      <c r="M11" s="56" t="s">
+      <c r="M11" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="73"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
-      <c r="R11" s="73"/>
-      <c r="S11" s="73"/>
-      <c r="T11" s="73"/>
-      <c r="U11" s="73"/>
-      <c r="V11" s="73"/>
-      <c r="W11" s="73"/>
-      <c r="X11" s="73"/>
-      <c r="Y11" s="73"/>
-      <c r="Z11" s="73"/>
-      <c r="AA11" s="73"/>
-      <c r="AB11" s="57"/>
-      <c r="AC11" s="74" t="s">
+      <c r="N11" s="77"/>
+      <c r="O11" s="77"/>
+      <c r="P11" s="77"/>
+      <c r="Q11" s="77"/>
+      <c r="R11" s="77"/>
+      <c r="S11" s="77"/>
+      <c r="T11" s="77"/>
+      <c r="U11" s="77"/>
+      <c r="V11" s="77"/>
+      <c r="W11" s="77"/>
+      <c r="X11" s="77"/>
+      <c r="Y11" s="77"/>
+      <c r="Z11" s="77"/>
+      <c r="AA11" s="77"/>
+      <c r="AB11" s="78"/>
+      <c r="AC11" s="79" t="s">
         <v>19</v>
       </c>
       <c r="AD11" s="16" t="s">
@@ -7870,75 +7868,75 @@
       <c r="AE11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="AF11" s="64" t="s">
+      <c r="AF11" s="84" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:39" s="20" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="65" t="s">
+      <c r="B12" s="84"/>
+      <c r="C12" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="67" t="s">
+      <c r="D12" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="67" t="s">
+      <c r="E12" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="68" t="s">
+      <c r="F12" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="67" t="s">
+      <c r="G12" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="67" t="s">
+      <c r="H12" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="I12" s="67" t="s">
+      <c r="I12" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="67" t="s">
+      <c r="J12" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="K12" s="65" t="s">
+      <c r="K12" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="L12" s="65" t="s">
+      <c r="L12" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="M12" s="70" t="s">
+      <c r="M12" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="N12" s="71"/>
-      <c r="O12" s="71"/>
-      <c r="P12" s="71"/>
-      <c r="Q12" s="71"/>
-      <c r="R12" s="71"/>
-      <c r="S12" s="72"/>
-      <c r="T12" s="70" t="s">
+      <c r="N12" s="74"/>
+      <c r="O12" s="74"/>
+      <c r="P12" s="74"/>
+      <c r="Q12" s="74"/>
+      <c r="R12" s="74"/>
+      <c r="S12" s="75"/>
+      <c r="T12" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="U12" s="71"/>
-      <c r="V12" s="71"/>
-      <c r="W12" s="71"/>
-      <c r="X12" s="72"/>
-      <c r="Y12" s="70" t="s">
+      <c r="U12" s="74"/>
+      <c r="V12" s="74"/>
+      <c r="W12" s="74"/>
+      <c r="X12" s="75"/>
+      <c r="Y12" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="Z12" s="71"/>
-      <c r="AA12" s="71"/>
-      <c r="AB12" s="72"/>
-      <c r="AC12" s="75"/>
+      <c r="Z12" s="74"/>
+      <c r="AA12" s="74"/>
+      <c r="AB12" s="75"/>
+      <c r="AC12" s="80"/>
       <c r="AD12" s="18" t="s">
         <v>75</v>
       </c>
       <c r="AE12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="AF12" s="64"/>
+      <c r="AF12" s="84"/>
     </row>
     <row r="13" spans="1:39" s="20" customFormat="1" ht="124.5" customHeight="1">
       <c r="A13" s="18" t="s">
@@ -7947,16 +7945,16 @@
       <c r="B13" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="66"/>
-      <c r="L13" s="66"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="89"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
       <c r="M13" s="21" t="s">
         <v>28</v>
       </c>
@@ -8005,14 +8003,14 @@
       <c r="AB13" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="AC13" s="76"/>
+      <c r="AC13" s="81"/>
       <c r="AD13" s="21" t="s">
         <v>44</v>
       </c>
       <c r="AE13" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="AF13" s="64"/>
+      <c r="AF13" s="84"/>
     </row>
     <row r="14" spans="1:39" s="20" customFormat="1" ht="20.25" customHeight="1">
       <c r="A14" s="22"/>
@@ -10404,43 +10402,43 @@
       <c r="D85" s="27"/>
       <c r="E85" s="27"/>
       <c r="F85" s="27"/>
-      <c r="H85" s="79" t="s">
+      <c r="H85" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="I85" s="80"/>
-      <c r="J85" s="80"/>
-      <c r="K85" s="80"/>
-      <c r="L85" s="60"/>
-      <c r="M85" s="61"/>
-      <c r="N85" s="62"/>
-      <c r="O85" s="63"/>
-      <c r="P85" s="63"/>
+      <c r="I85" s="52"/>
+      <c r="J85" s="52"/>
+      <c r="K85" s="52"/>
+      <c r="L85" s="53"/>
+      <c r="M85" s="54"/>
+      <c r="N85" s="55"/>
+      <c r="O85" s="56"/>
+      <c r="P85" s="56"/>
       <c r="Q85" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R85" s="30"/>
-      <c r="S85" s="94" t="s">
+      <c r="S85" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="T85" s="95"/>
-      <c r="U85" s="95"/>
-      <c r="V85" s="95"/>
-      <c r="W85" s="95"/>
-      <c r="X85" s="96"/>
-      <c r="Y85" s="94" t="s">
+      <c r="T85" s="58"/>
+      <c r="U85" s="58"/>
+      <c r="V85" s="58"/>
+      <c r="W85" s="58"/>
+      <c r="X85" s="59"/>
+      <c r="Y85" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="Z85" s="95"/>
-      <c r="AA85" s="96"/>
-      <c r="AB85" s="93" t="s">
+      <c r="Z85" s="58"/>
+      <c r="AA85" s="59"/>
+      <c r="AB85" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="AC85" s="93"/>
-      <c r="AD85" s="93"/>
-      <c r="AE85" s="77" t="s">
+      <c r="AC85" s="72"/>
+      <c r="AD85" s="72"/>
+      <c r="AE85" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="AF85" s="78"/>
+      <c r="AF85" s="83"/>
     </row>
     <row r="86" spans="1:32" s="28" customFormat="1" ht="17.25" customHeight="1">
       <c r="A86" s="26"/>
@@ -10450,167 +10448,176 @@
       <c r="E86" s="27"/>
       <c r="F86" s="27"/>
       <c r="G86" s="32"/>
-      <c r="H86" s="79" t="s">
+      <c r="H86" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="I86" s="80"/>
-      <c r="J86" s="80"/>
-      <c r="K86" s="80"/>
-      <c r="L86" s="60"/>
-      <c r="M86" s="61"/>
-      <c r="N86" s="62"/>
-      <c r="O86" s="63"/>
-      <c r="P86" s="63"/>
+      <c r="I86" s="52"/>
+      <c r="J86" s="52"/>
+      <c r="K86" s="52"/>
+      <c r="L86" s="53"/>
+      <c r="M86" s="54"/>
+      <c r="N86" s="55"/>
+      <c r="O86" s="56"/>
+      <c r="P86" s="56"/>
       <c r="Q86" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R86" s="30"/>
-      <c r="S86" s="81" t="s">
+      <c r="S86" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="T86" s="82"/>
-      <c r="U86" s="82"/>
-      <c r="V86" s="82"/>
-      <c r="W86" s="82"/>
-      <c r="X86" s="83"/>
-      <c r="Y86" s="87"/>
-      <c r="Z86" s="88"/>
-      <c r="AA86" s="89"/>
-      <c r="AB86" s="93"/>
-      <c r="AC86" s="93"/>
-      <c r="AD86" s="93"/>
+      <c r="T86" s="61"/>
+      <c r="U86" s="61"/>
+      <c r="V86" s="61"/>
+      <c r="W86" s="61"/>
+      <c r="X86" s="62"/>
+      <c r="Y86" s="66"/>
+      <c r="Z86" s="67"/>
+      <c r="AA86" s="68"/>
+      <c r="AB86" s="72"/>
+      <c r="AC86" s="72"/>
+      <c r="AD86" s="72"/>
       <c r="AE86" s="33"/>
       <c r="AF86" s="34"/>
     </row>
     <row r="87" spans="1:32" s="28" customFormat="1" ht="17.25" customHeight="1">
-      <c r="H87" s="79" t="s">
+      <c r="H87" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="I87" s="80"/>
-      <c r="J87" s="80"/>
-      <c r="K87" s="80"/>
-      <c r="L87" s="60"/>
-      <c r="M87" s="61"/>
-      <c r="N87" s="62"/>
-      <c r="O87" s="63"/>
-      <c r="P87" s="63"/>
+      <c r="I87" s="52"/>
+      <c r="J87" s="52"/>
+      <c r="K87" s="52"/>
+      <c r="L87" s="53"/>
+      <c r="M87" s="54"/>
+      <c r="N87" s="55"/>
+      <c r="O87" s="56"/>
+      <c r="P87" s="56"/>
       <c r="Q87" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R87" s="30"/>
-      <c r="S87" s="84"/>
-      <c r="T87" s="85"/>
-      <c r="U87" s="85"/>
-      <c r="V87" s="85"/>
-      <c r="W87" s="85"/>
-      <c r="X87" s="86"/>
-      <c r="Y87" s="90"/>
-      <c r="Z87" s="91"/>
-      <c r="AA87" s="92"/>
-      <c r="AB87" s="93"/>
-      <c r="AC87" s="93"/>
-      <c r="AD87" s="93"/>
+      <c r="S87" s="63"/>
+      <c r="T87" s="64"/>
+      <c r="U87" s="64"/>
+      <c r="V87" s="64"/>
+      <c r="W87" s="64"/>
+      <c r="X87" s="65"/>
+      <c r="Y87" s="69"/>
+      <c r="Z87" s="70"/>
+      <c r="AA87" s="71"/>
+      <c r="AB87" s="72"/>
+      <c r="AC87" s="72"/>
+      <c r="AD87" s="72"/>
     </row>
     <row r="88" spans="1:32" s="28" customFormat="1" ht="17.25" customHeight="1">
       <c r="A88" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="H88" s="79" t="s">
+      <c r="H88" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="I88" s="80"/>
-      <c r="J88" s="80"/>
-      <c r="K88" s="80"/>
-      <c r="L88" s="60"/>
-      <c r="M88" s="61"/>
-      <c r="N88" s="62"/>
-      <c r="O88" s="63"/>
-      <c r="P88" s="63"/>
+      <c r="I88" s="52"/>
+      <c r="J88" s="52"/>
+      <c r="K88" s="52"/>
+      <c r="L88" s="53"/>
+      <c r="M88" s="54"/>
+      <c r="N88" s="55"/>
+      <c r="O88" s="56"/>
+      <c r="P88" s="56"/>
       <c r="Q88" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R88" s="30"/>
-      <c r="S88" s="81" t="s">
+      <c r="S88" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="T88" s="82"/>
-      <c r="U88" s="82"/>
-      <c r="V88" s="82"/>
-      <c r="W88" s="82"/>
-      <c r="X88" s="83"/>
-      <c r="Y88" s="87"/>
-      <c r="Z88" s="88"/>
-      <c r="AA88" s="89"/>
-      <c r="AB88" s="93"/>
-      <c r="AC88" s="93"/>
-      <c r="AD88" s="93"/>
+      <c r="T88" s="61"/>
+      <c r="U88" s="61"/>
+      <c r="V88" s="61"/>
+      <c r="W88" s="61"/>
+      <c r="X88" s="62"/>
+      <c r="Y88" s="66"/>
+      <c r="Z88" s="67"/>
+      <c r="AA88" s="68"/>
+      <c r="AB88" s="72"/>
+      <c r="AC88" s="72"/>
+      <c r="AD88" s="72"/>
     </row>
     <row r="89" spans="1:32" s="28" customFormat="1" ht="17.25" customHeight="1">
       <c r="A89" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="H89" s="79" t="s">
+      <c r="H89" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="I89" s="80"/>
-      <c r="J89" s="80"/>
-      <c r="K89" s="80"/>
-      <c r="L89" s="60"/>
-      <c r="M89" s="61"/>
-      <c r="N89" s="62"/>
-      <c r="O89" s="63"/>
-      <c r="P89" s="63"/>
+      <c r="I89" s="52"/>
+      <c r="J89" s="52"/>
+      <c r="K89" s="52"/>
+      <c r="L89" s="53"/>
+      <c r="M89" s="54"/>
+      <c r="N89" s="55"/>
+      <c r="O89" s="56"/>
+      <c r="P89" s="56"/>
       <c r="Q89" s="29" t="s">
         <v>46</v>
       </c>
       <c r="R89" s="30"/>
-      <c r="S89" s="84"/>
-      <c r="T89" s="85"/>
-      <c r="U89" s="85"/>
-      <c r="V89" s="85"/>
-      <c r="W89" s="85"/>
-      <c r="X89" s="86"/>
-      <c r="Y89" s="90"/>
-      <c r="Z89" s="91"/>
-      <c r="AA89" s="92"/>
-      <c r="AB89" s="93"/>
-      <c r="AC89" s="93"/>
-      <c r="AD89" s="93"/>
+      <c r="S89" s="63"/>
+      <c r="T89" s="64"/>
+      <c r="U89" s="64"/>
+      <c r="V89" s="64"/>
+      <c r="W89" s="64"/>
+      <c r="X89" s="65"/>
+      <c r="Y89" s="69"/>
+      <c r="Z89" s="70"/>
+      <c r="AA89" s="71"/>
+      <c r="AB89" s="72"/>
+      <c r="AC89" s="72"/>
+      <c r="AD89" s="72"/>
     </row>
     <row r="90" spans="1:32" s="28" customFormat="1" ht="14.25"/>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="AE85:AF85"/>
-    <mergeCell ref="S86:X87"/>
-    <mergeCell ref="Y86:AA87"/>
-    <mergeCell ref="AB86:AD87"/>
-    <mergeCell ref="S88:X89"/>
-    <mergeCell ref="Y88:AA89"/>
-    <mergeCell ref="AB88:AD89"/>
-    <mergeCell ref="Y12:AB12"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="H89:K89"/>
-    <mergeCell ref="L89:M89"/>
-    <mergeCell ref="N89:P89"/>
-    <mergeCell ref="H86:K86"/>
-    <mergeCell ref="L86:M86"/>
-    <mergeCell ref="N86:P86"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="A3:AF3"/>
+    <mergeCell ref="A4:AF4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AE8:AF8"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="D6:H7"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="AB6:AD6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="N7:O8"/>
+    <mergeCell ref="P7:Q8"/>
+    <mergeCell ref="R7:S8"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="AE7:AF7"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="T7:U8"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="M11:AB11"/>
+    <mergeCell ref="V7:W8"/>
+    <mergeCell ref="AB7:AD7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="AB8:AD8"/>
     <mergeCell ref="AC11:AC13"/>
     <mergeCell ref="AB9:AD9"/>
-    <mergeCell ref="AF11:AF13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="M12:S12"/>
-    <mergeCell ref="T12:X12"/>
     <mergeCell ref="AE9:AF9"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
@@ -10627,44 +10634,35 @@
     <mergeCell ref="H85:K85"/>
     <mergeCell ref="L85:M85"/>
     <mergeCell ref="N85:P85"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="T7:U8"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="M11:AB11"/>
-    <mergeCell ref="V7:W8"/>
-    <mergeCell ref="AB7:AD7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="AB8:AD8"/>
-    <mergeCell ref="AE8:AF8"/>
-    <mergeCell ref="A6:C7"/>
-    <mergeCell ref="D6:H7"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="AB6:AD6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="N7:O8"/>
-    <mergeCell ref="P7:Q8"/>
-    <mergeCell ref="R7:S8"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="AE7:AF7"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="A3:AF3"/>
-    <mergeCell ref="A4:AF4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AF11:AF13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="M12:S12"/>
+    <mergeCell ref="T12:X12"/>
+    <mergeCell ref="Y12:AB12"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="H89:K89"/>
+    <mergeCell ref="L89:M89"/>
+    <mergeCell ref="N89:P89"/>
+    <mergeCell ref="H86:K86"/>
+    <mergeCell ref="L86:M86"/>
+    <mergeCell ref="N86:P86"/>
+    <mergeCell ref="AE85:AF85"/>
+    <mergeCell ref="S86:X87"/>
+    <mergeCell ref="Y86:AA87"/>
+    <mergeCell ref="AB86:AD87"/>
+    <mergeCell ref="S88:X89"/>
+    <mergeCell ref="Y88:AA89"/>
+    <mergeCell ref="AB88:AD89"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A85:K89 AC8:AD9 A3:AF4 J6:K9 A11:E13 G11:H11 J11:K11 F12:AB13 M11:AB11 Q85:AF89 AC11:AF13 A1:AE2 A8:C9 B5:C5 A5:A6 AB6:AB9 AC6:AD6 N6:N7 P6:W7 O6" xr:uid="{BE6BE2B8-BD32-4921-88BF-B5454DF6F2D3}">

</xml_diff>